<commit_message>
Atualização da distribuição de Tarefas.  (Participação do grupo inteiro)
</commit_message>
<xml_diff>
--- a/Distribuição de tarefas.xlsx
+++ b/Distribuição de tarefas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="53">
   <si>
     <t>3D</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -371,6 +374,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -389,44 +425,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -731,21 +734,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:J50"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="28.85546875" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" style="21" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" style="4" customWidth="1"/>
     <col min="5" max="10" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="9"/>
+      <c r="D2" s="3"/>
       <c r="E2" s="1" t="s">
         <v>46</v>
       </c>
@@ -764,13 +767,13 @@
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="2"/>
@@ -789,9 +792,9 @@
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="9" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="2"/>
@@ -810,9 +813,9 @@
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="16"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="9" t="s">
+      <c r="B5" s="6"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="2"/>
@@ -831,9 +834,9 @@
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="16"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="9" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="2"/>
@@ -852,9 +855,9 @@
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="16"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="9" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="2"/>
@@ -873,9 +876,9 @@
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="16"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="9" t="s">
+      <c r="B8" s="6"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="2"/>
@@ -894,9 +897,9 @@
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="16"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="9" t="s">
+      <c r="B9" s="6"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="2"/>
@@ -915,9 +918,9 @@
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="16"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="9" t="s">
+      <c r="B10" s="6"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="2"/>
@@ -936,9 +939,9 @@
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="16"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="9" t="s">
+      <c r="B11" s="6"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="2"/>
@@ -957,22 +960,22 @@
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="16"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="20"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="13"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="16"/>
-      <c r="C13" s="12" t="s">
+      <c r="B13" s="6"/>
+      <c r="C13" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="2"/>
@@ -989,9 +992,9 @@
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="16"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="9" t="s">
+      <c r="B14" s="6"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E14" s="2"/>
@@ -1008,9 +1011,9 @@
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="16"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="9" t="s">
+      <c r="B15" s="6"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E15" s="2"/>
@@ -1027,20 +1030,20 @@
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="16"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="20"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="13"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="16"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="9" t="s">
+      <c r="B17" s="6"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E17" s="2"/>
@@ -1057,20 +1060,20 @@
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="16"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="20"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="13"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="16"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="9" t="s">
+      <c r="B19" s="6"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E19" s="2"/>
@@ -1087,33 +1090,33 @@
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="16"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="20"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="13"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="17"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="20"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="13"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="9" t="s">
+      <c r="C22" s="8"/>
+      <c r="D22" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E22" s="2"/>
@@ -1132,9 +1135,9 @@
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="9" t="s">
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E23" s="2"/>
@@ -1153,9 +1156,9 @@
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="9" t="s">
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E24" s="2"/>
@@ -1174,9 +1177,9 @@
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="9" t="s">
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E25" s="2"/>
@@ -1195,22 +1198,22 @@
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="13"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="20"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="13"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="13"/>
-      <c r="C27" s="12" t="s">
+      <c r="B27" s="9"/>
+      <c r="C27" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E27" s="2"/>
@@ -1229,24 +1232,24 @@
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="20"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="13"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D29" s="3" t="s">
         <v>26</v>
       </c>
       <c r="E29" s="2" t="s">
@@ -1259,13 +1262,13 @@
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="9" t="s">
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E30" s="2" t="s">
@@ -1277,25 +1280,23 @@
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
-      <c r="J30" s="2" t="s">
-        <v>51</v>
-      </c>
+      <c r="J30" s="2"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="20"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="13"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="9" t="s">
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E32" s="2" t="s">
@@ -1307,27 +1308,25 @@
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
-      <c r="J32" s="2" t="s">
-        <v>51</v>
-      </c>
+      <c r="J32" s="2"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="13"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="20"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="13"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="13"/>
-      <c r="C34" s="12" t="s">
+      <c r="B34" s="9"/>
+      <c r="C34" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="D34" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E34" s="2" t="s">
@@ -1339,14 +1338,12 @@
       </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
-      <c r="J34" s="2" t="s">
-        <v>51</v>
-      </c>
+      <c r="J34" s="2"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="9" t="s">
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E35" s="2" t="s">
@@ -1358,14 +1355,12 @@
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
-      <c r="J35" s="2" t="s">
-        <v>51</v>
-      </c>
+      <c r="J35" s="2"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="9" t="s">
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E36" s="2" t="s">
@@ -1377,14 +1372,12 @@
       </c>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
-      <c r="J36" s="2" t="s">
-        <v>51</v>
-      </c>
+      <c r="J36" s="2"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="9" t="s">
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E37" s="2" t="s">
@@ -1396,25 +1389,23 @@
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
-      <c r="J37" s="2" t="s">
-        <v>51</v>
-      </c>
+      <c r="J37" s="2"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
-      <c r="I38" s="19"/>
-      <c r="J38" s="20"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="13"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="9" t="s">
+      <c r="B39" s="9"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E39" s="2" t="s">
@@ -1426,14 +1417,12 @@
       </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
-      <c r="J39" s="2" t="s">
-        <v>51</v>
-      </c>
+      <c r="J39" s="2"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="9" t="s">
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E40" s="2" t="s">
@@ -1445,14 +1434,12 @@
       </c>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
-      <c r="J40" s="2" t="s">
-        <v>51</v>
-      </c>
+      <c r="J40" s="2"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="9" t="s">
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="3" t="s">
         <v>36</v>
       </c>
       <c r="E41" s="2" t="s">
@@ -1464,14 +1451,12 @@
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
-      <c r="J41" s="2" t="s">
-        <v>51</v>
-      </c>
+      <c r="J41" s="2"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="13"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="9" t="s">
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E42" s="2" t="s">
@@ -1483,27 +1468,25 @@
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
-      <c r="J42" s="2" t="s">
-        <v>51</v>
-      </c>
+      <c r="J42" s="2"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="19"/>
-      <c r="H43" s="19"/>
-      <c r="I43" s="19"/>
-      <c r="J43" s="20"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="12"/>
+      <c r="I43" s="12"/>
+      <c r="J43" s="13"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C44" s="4"/>
-      <c r="D44" s="9" t="s">
+      <c r="C44" s="15"/>
+      <c r="D44" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E44" s="2" t="s">
@@ -1518,9 +1501,9 @@
       <c r="J44" s="2"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B45" s="5"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="9" t="s">
+      <c r="B45" s="16"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E45" s="2" t="s">
@@ -1535,22 +1518,22 @@
       <c r="J45" s="2"/>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B46" s="7"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="19"/>
-      <c r="G46" s="19"/>
-      <c r="H46" s="19"/>
-      <c r="I46" s="19"/>
-      <c r="J46" s="20"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="13"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C47" s="4"/>
-      <c r="D47" s="9" t="s">
+      <c r="C47" s="15"/>
+      <c r="D47" s="3" t="s">
         <v>43</v>
       </c>
       <c r="E47" s="2" t="s">
@@ -1573,9 +1556,9 @@
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B48" s="5"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="9" t="s">
+      <c r="B48" s="16"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E48" s="2" t="s">
@@ -1598,22 +1581,22 @@
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B49" s="7"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="19"/>
-      <c r="G49" s="19"/>
-      <c r="H49" s="19"/>
-      <c r="I49" s="19"/>
-      <c r="J49" s="20"/>
+      <c r="B49" s="18"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="12"/>
+      <c r="I49" s="12"/>
+      <c r="J49" s="13"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B50" s="10" t="s">
+      <c r="B50" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="C50" s="11"/>
-      <c r="D50" s="9" t="s">
+      <c r="C50" s="21"/>
+      <c r="D50" s="3" t="s">
         <v>45</v>
       </c>
       <c r="E50" s="2" t="s">
@@ -1637,15 +1620,12 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B3:B21"/>
-    <mergeCell ref="B22:B28"/>
-    <mergeCell ref="B29:B43"/>
-    <mergeCell ref="C22:C26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C29:C33"/>
-    <mergeCell ref="C34:C43"/>
-    <mergeCell ref="C13:C21"/>
-    <mergeCell ref="C3:C12"/>
+    <mergeCell ref="D43:J43"/>
+    <mergeCell ref="B44:C46"/>
+    <mergeCell ref="B47:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D49:J49"/>
+    <mergeCell ref="D46:J46"/>
     <mergeCell ref="D20:J20"/>
     <mergeCell ref="D18:J18"/>
     <mergeCell ref="D16:J16"/>
@@ -1656,12 +1636,15 @@
     <mergeCell ref="D33:J33"/>
     <mergeCell ref="D26:J26"/>
     <mergeCell ref="D21:J21"/>
-    <mergeCell ref="B44:C46"/>
-    <mergeCell ref="B47:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D49:J49"/>
-    <mergeCell ref="D46:J46"/>
-    <mergeCell ref="D43:J43"/>
+    <mergeCell ref="B3:B21"/>
+    <mergeCell ref="B22:B28"/>
+    <mergeCell ref="B29:B43"/>
+    <mergeCell ref="C22:C26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C33"/>
+    <mergeCell ref="C34:C43"/>
+    <mergeCell ref="C13:C21"/>
+    <mergeCell ref="C3:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
atualização da tabela de distribuição de tarefas, agora sem o Bruno. close issues #1
</commit_message>
<xml_diff>
--- a/Distribuição de tarefas.xlsx
+++ b/Distribuição de tarefas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="53">
   <si>
     <t>3D</t>
   </si>
@@ -162,9 +162,6 @@
     <t>José Fontoura</t>
   </si>
   <si>
-    <t>Roberto DuarteBruno Costa</t>
-  </si>
-  <si>
     <t>Jorge Tavares</t>
   </si>
   <si>
@@ -175,6 +172,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Roberto Duarte</t>
   </si>
 </sst>
 </file>
@@ -380,6 +380,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -396,39 +429,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -732,20 +732,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J50"/>
+  <dimension ref="B2:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="28.85546875" customWidth="1"/>
     <col min="4" max="4" width="30.7109375" style="4" customWidth="1"/>
-    <col min="5" max="10" width="13.7109375" customWidth="1"/>
+    <col min="5" max="9" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="3"/>
@@ -756,21 +756,20 @@
         <v>47</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="19" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -778,201 +777,173 @@
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="6"/>
-      <c r="C4" s="9"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="17"/>
+      <c r="C4" s="20"/>
       <c r="D4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="6"/>
-      <c r="C5" s="9"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="17"/>
+      <c r="C5" s="20"/>
       <c r="D5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
-      <c r="C6" s="9"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="17"/>
+      <c r="C6" s="20"/>
       <c r="D6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="6"/>
-      <c r="C7" s="9"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="17"/>
+      <c r="C7" s="20"/>
       <c r="D7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="6"/>
-      <c r="C8" s="9"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="17"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="6"/>
-      <c r="C9" s="9"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="17"/>
+      <c r="C9" s="20"/>
       <c r="D9" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
-      <c r="C10" s="9"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="17"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="6"/>
-      <c r="C11" s="9"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="17"/>
+      <c r="C11" s="20"/>
       <c r="D11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="13"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="6"/>
-      <c r="C13" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="17"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="7"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="17"/>
+      <c r="C13" s="19" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -982,18 +953,15 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="6"/>
-      <c r="C14" s="9"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="17"/>
+      <c r="C14" s="20"/>
       <c r="D14" s="3" t="s">
         <v>12</v>
       </c>
@@ -1001,18 +969,15 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="6"/>
-      <c r="C15" s="9"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="17"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="3" t="s">
         <v>13</v>
       </c>
@@ -1020,29 +985,25 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="6"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="13"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="6"/>
-      <c r="C17" s="9"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="17"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="7"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="17"/>
+      <c r="C17" s="20"/>
       <c r="D17" s="3" t="s">
         <v>15</v>
       </c>
@@ -1050,29 +1011,25 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="6"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="13"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="6"/>
-      <c r="C19" s="9"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="17"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="7"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="17"/>
+      <c r="C19" s="20"/>
       <c r="D19" s="3" t="s">
         <v>21</v>
       </c>
@@ -1080,137 +1037,119 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="6"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="13"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="7"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="13"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="17"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="7"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="18"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="8"/>
+      <c r="C22" s="19"/>
       <c r="D22" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
       <c r="D23" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
       <c r="D24" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
       <c r="D25" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="9"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="13"/>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="9"/>
-      <c r="C27" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="20"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="7"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="20"/>
+      <c r="C27" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D27" s="3" t="s">
@@ -1219,423 +1158,375 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="13"/>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="7"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="19" t="s">
         <v>25</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>26</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
       <c r="D30" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="13"/>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="7"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
       <c r="D32" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="9"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="13"/>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="9"/>
-      <c r="C34" s="8" t="s">
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="20"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="7"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="20"/>
+      <c r="C34" s="19" t="s">
         <v>29</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
       <c r="D35" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
       <c r="D36" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="9"/>
-      <c r="C37" s="9"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="20"/>
+      <c r="C37" s="20"/>
       <c r="D37" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
-      <c r="I38" s="12"/>
-      <c r="J38" s="13"/>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="20"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="7"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="20"/>
+      <c r="C39" s="20"/>
       <c r="D39" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
       <c r="D40" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F40" s="2"/>
       <c r="G40" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
       <c r="D41" s="3" t="s">
         <v>36</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F41" s="2"/>
       <c r="G41" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
       <c r="D42" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="12"/>
-      <c r="H43" s="12"/>
-      <c r="I43" s="12"/>
-      <c r="J43" s="13"/>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B44" s="14" t="s">
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="21"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="7"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C44" s="15"/>
+      <c r="C44" s="9"/>
       <c r="D44" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B45" s="16"/>
-      <c r="C45" s="17"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="10"/>
+      <c r="C45" s="11"/>
       <c r="D45" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B46" s="18"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
-      <c r="H46" s="12"/>
-      <c r="I46" s="12"/>
-      <c r="J46" s="13"/>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B47" s="14" t="s">
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="12"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="7"/>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B47" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C47" s="15"/>
+      <c r="C47" s="9"/>
       <c r="D47" s="3" t="s">
         <v>43</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J47" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B48" s="16"/>
-      <c r="C48" s="17"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B48" s="10"/>
+      <c r="C48" s="11"/>
       <c r="D48" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B49" s="18"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="12"/>
-      <c r="F49" s="12"/>
-      <c r="G49" s="12"/>
-      <c r="H49" s="12"/>
-      <c r="I49" s="12"/>
-      <c r="J49" s="13"/>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B50" s="20" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B49" s="12"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="7"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B50" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C50" s="21"/>
+      <c r="C50" s="15"/>
       <c r="D50" s="3" t="s">
         <v>45</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J50" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="D43:J43"/>
-    <mergeCell ref="B44:C46"/>
-    <mergeCell ref="B47:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D49:J49"/>
-    <mergeCell ref="D46:J46"/>
-    <mergeCell ref="D20:J20"/>
-    <mergeCell ref="D18:J18"/>
-    <mergeCell ref="D16:J16"/>
-    <mergeCell ref="D12:J12"/>
-    <mergeCell ref="D38:J38"/>
-    <mergeCell ref="D28:J28"/>
-    <mergeCell ref="D31:J31"/>
-    <mergeCell ref="D33:J33"/>
-    <mergeCell ref="D26:J26"/>
-    <mergeCell ref="D21:J21"/>
     <mergeCell ref="B3:B21"/>
     <mergeCell ref="B22:B28"/>
     <mergeCell ref="B29:B43"/>
@@ -1645,6 +1536,22 @@
     <mergeCell ref="C34:C43"/>
     <mergeCell ref="C13:C21"/>
     <mergeCell ref="C3:C12"/>
+    <mergeCell ref="D20:I20"/>
+    <mergeCell ref="D18:I18"/>
+    <mergeCell ref="D16:I16"/>
+    <mergeCell ref="D12:I12"/>
+    <mergeCell ref="D38:I38"/>
+    <mergeCell ref="D28:I28"/>
+    <mergeCell ref="D31:I31"/>
+    <mergeCell ref="D33:I33"/>
+    <mergeCell ref="D26:I26"/>
+    <mergeCell ref="D21:I21"/>
+    <mergeCell ref="D43:I43"/>
+    <mergeCell ref="B44:C46"/>
+    <mergeCell ref="B47:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D49:I49"/>
+    <mergeCell ref="D46:I46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>